<commit_message>
Various updates for the back panel and bom
added the new rear panel for the top hat as well as redesigned the hinge stops to allow for a backpanel and updated the bom to include the new screws and nuts for the back panel
</commit_message>
<xml_diff>
--- a/printer_mods/hartk1213/Voron0_Hinged_Top_Hat/BOM/Voron0_Hinged_Top_Hat_BOM.xlsx
+++ b/printer_mods/hartk1213/Voron0_Hinged_Top_Hat/BOM/Voron0_Hinged_Top_Hat_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\User Folders\Documents\3D Printer\Printers\Voron\VoronUsers\printer_mods\hartk1213\Voron0_Hinged_Top_Hat\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC80719B-6DF7-4758-8763-34FBB83F4216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670D3CEF-672B-4A9C-9227-0C87BA50F825}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30705" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,8 +381,8 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -604,8 +604,8 @@
         <v>21</v>
       </c>
       <c r="B19" s="3">
-        <f>62</f>
-        <v>62</v>
+        <f>62+6</f>
+        <v>68</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -652,8 +652,8 @@
         <v>25</v>
       </c>
       <c r="B23" s="3">
-        <f>58</f>
-        <v>58</v>
+        <f>58+6</f>
+        <v>64</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>

</xml_diff>